<commit_message>
updated lab calculations and records now working
</commit_message>
<xml_diff>
--- a/mice_records/mouse_organs.xlsx
+++ b/mice_records/mouse_organs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>Mouse no</t>
   </si>
@@ -47,15 +47,53 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>AVI345</t>
+  </si>
+  <si>
+    <t>AV234</t>
+  </si>
+  <si>
+    <t>AVI456</t>
+  </si>
+  <si>
+    <t>AV457</t>
+  </si>
+  <si>
+    <t>AV567</t>
+  </si>
+  <si>
+    <t>AVI321</t>
+  </si>
+  <si>
+    <t>456</t>
+  </si>
+  <si>
+    <t>AV789</t>
+  </si>
+  <si>
+    <t>AV569</t>
+  </si>
+  <si>
+    <t>AV345</t>
+  </si>
+  <si>
+    <t>AVI213</t>
+  </si>
+  <si>
+    <t>AVI989</t>
+  </si>
+  <si>
+    <t>AV678</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="yyyy\-mm\-dd\ h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="165"/>
+  <numFmts count="1">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -88,8 +126,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -365,19 +403,22 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H4"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="1" width="10.7109375"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -400,20 +441,89 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="B2" s="1" t="n"/>
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>43012</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="B3" s="1" t="n"/>
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="B4" s="1" t="n"/>
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>43012</v>
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>43013</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -431,6 +541,396 @@
         <v>10</v>
       </c>
       <c r="H5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>43013</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>